<commit_message>
initial commit of full file set to a new repo
</commit_message>
<xml_diff>
--- a/work_out_files/metrics_file.xlsx
+++ b/work_out_files/metrics_file.xlsx
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8375286041189931</v>
+        <v>0.8268497330282227</v>
       </c>
       <c r="D2" t="n">
-        <v>0.830137567638939</v>
+        <v>0.8177987028702338</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8375286041189931</v>
+        <v>0.8268497330282227</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8223752214706125</v>
+        <v>0.8123177461656231</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9080854309687262</v>
+        <v>0.9077040427154843</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9033159174563196</v>
+        <v>0.903320740687993</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9080854309687262</v>
+        <v>0.9077040427154843</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9014633780570762</v>
+        <v>0.9008123345596354</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9959954233409611</v>
+        <v>0.9944698703279939</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9960114599751793</v>
+        <v>0.9945004526621831</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9959954233409611</v>
+        <v>0.9944698703279939</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9939971522135932</v>
+        <v>0.9917124722746894</v>
       </c>
     </row>
     <row r="5">
@@ -536,16 +536,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.7791762013729977</v>
+        <v>0.7864225781845919</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7778073184435872</v>
+        <v>0.7872906718385223</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7791762013729977</v>
+        <v>0.7864225781845919</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7768471823643884</v>
+        <v>0.7831637240824391</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.933066361556064</v>
+        <v>0.9189549961861174</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9195802350177146</v>
+        <v>0.8992381992068549</v>
       </c>
       <c r="E6" t="n">
-        <v>0.933066361556064</v>
+        <v>0.9189549961861174</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9143354502992973</v>
+        <v>0.8945725637734619</v>
       </c>
     </row>
     <row r="7">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9527078565980168</v>
+        <v>0.9551868802440885</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9464978278504006</v>
+        <v>0.9472949768923256</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9527078565980168</v>
+        <v>0.9551868802440885</v>
       </c>
       <c r="F7" t="n">
-        <v>0.937097180561184</v>
+        <v>0.9419755365761606</v>
       </c>
     </row>
     <row r="8">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9704424103737604</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9640851139706974</v>
+        <v>0.964893852277753</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9704424103737604</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9572957671642613</v>
+        <v>0.9621167640204594</v>
       </c>
     </row>
     <row r="9">
@@ -624,16 +624,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9836003051106026</v>
+        <v>0.9794050343249427</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9838692551030679</v>
+        <v>0.9798291869360995</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9836003051106026</v>
+        <v>0.9794050343249427</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9754682510595054</v>
+        <v>0.9692146929273422</v>
       </c>
     </row>
     <row r="10">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9654843630816171</v>
+        <v>0.9662471395881007</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9518696494835303</v>
+        <v>0.9586968623059617</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9654843630816171</v>
+        <v>0.9662471395881007</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9520672793097094</v>
+        <v>0.9544755771023257</v>
       </c>
     </row>
     <row r="11">
@@ -668,16 +668,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9612890922959573</v>
+        <v>0.9610983981693364</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9572450669015721</v>
+        <v>0.9576300588995028</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9612890922959573</v>
+        <v>0.9610983981693364</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9574124397570783</v>
+        <v>0.9569191488828531</v>
       </c>
     </row>
     <row r="12">
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9406941266209001</v>
+        <v>0.9464149504195271</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9366306539639554</v>
+        <v>0.9438230591104911</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9406941266209001</v>
+        <v>0.9464149504195271</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9367901536652637</v>
+        <v>0.942051978867804</v>
       </c>
     </row>
     <row r="13">
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9441266209000763</v>
+        <v>0.9427917620137299</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9394307573796159</v>
+        <v>0.9386830439089836</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9441266209000763</v>
+        <v>0.9427917620137299</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9359965319049026</v>
+        <v>0.934549663266837</v>
       </c>
     </row>
     <row r="14">
@@ -734,16 +734,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9858886346300534</v>
+        <v>0.9856979405034325</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9821814034766304</v>
+        <v>0.9824567065882263</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9858886346300534</v>
+        <v>0.9856979405034325</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9819931443009149</v>
+        <v>0.981738016480412</v>
       </c>
     </row>
     <row r="15">
@@ -756,16 +756,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9794050343249427</v>
+        <v>0.9792143401983219</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9769738170348974</v>
+        <v>0.9731808319745648</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9794050343249427</v>
+        <v>0.9792143401983219</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9713952783708385</v>
+        <v>0.970918224366996</v>
       </c>
     </row>
     <row r="16">
@@ -778,16 +778,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9889397406559878</v>
+        <v>0.9893211289092296</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9890620933246798</v>
+        <v>0.9894351671970029</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9889397406559878</v>
+        <v>0.9893211289092296</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9836247069367018</v>
+        <v>0.9840103559779684</v>
       </c>
     </row>
     <row r="17">
@@ -800,16 +800,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9683447749809306</v>
+        <v>0.9679633867276888</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9636961223913156</v>
+        <v>0.9603865694003006</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9683447749809306</v>
+        <v>0.9679633867276888</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9546584369122239</v>
+        <v>0.9555857458440002</v>
       </c>
     </row>
     <row r="18">
@@ -822,16 +822,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.9635774218154081</v>
+        <v>0.9607170099160945</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9595406342698973</v>
+        <v>0.9589298282463142</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9635774218154081</v>
+        <v>0.9607170099160945</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9533977106879298</v>
+        <v>0.9496149427735556</v>
       </c>
     </row>
     <row r="19">
@@ -844,16 +844,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.873951182303585</v>
+        <v>0.8728070175438597</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8497714072831241</v>
+        <v>0.8409987613237453</v>
       </c>
       <c r="E19" t="n">
-        <v>0.873951182303585</v>
+        <v>0.8728070175438597</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8338823737611161</v>
+        <v>0.8327191554311399</v>
       </c>
     </row>
     <row r="20">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.936880244088482</v>
+        <v>0.9364988558352403</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9171196594819329</v>
+        <v>0.9256431109179933</v>
       </c>
       <c r="E20" t="n">
-        <v>0.936880244088482</v>
+        <v>0.9364988558352403</v>
       </c>
       <c r="F20" t="n">
-        <v>0.909526059240098</v>
+        <v>0.9100347432995428</v>
       </c>
     </row>
     <row r="21">
@@ -888,16 +888,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9607170099160945</v>
+        <v>0.9586193745232647</v>
       </c>
       <c r="D21" t="n">
-        <v>0.957308156077583</v>
+        <v>0.9528569127537951</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9607170099160945</v>
+        <v>0.9586193745232647</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9461394883048011</v>
+        <v>0.9438677719481351</v>
       </c>
     </row>
     <row r="22">
@@ -910,16 +910,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.9588100686498856</v>
+        <v>0.9582379862700229</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9514530315340987</v>
+        <v>0.9539325831904284</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9588100686498856</v>
+        <v>0.9582379862700229</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9489774683228951</v>
+        <v>0.9469725454799259</v>
       </c>
     </row>
     <row r="23">
@@ -932,16 +932,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.9807398932112891</v>
+        <v>0.9811212814645309</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9768986837335316</v>
+        <v>0.9754349468428717</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9807398932112891</v>
+        <v>0.9811212814645309</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9732673543363756</v>
+        <v>0.9746755561320826</v>
       </c>
     </row>
     <row r="24">
@@ -954,16 +954,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.9931350114416476</v>
+        <v>0.994279176201373</v>
       </c>
       <c r="D24" t="n">
-        <v>0.993182139509554</v>
+        <v>0.9943119040263079</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9931350114416476</v>
+        <v>0.994279176201373</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9897143397604479</v>
+        <v>0.9914269697291946</v>
       </c>
     </row>
     <row r="25">
@@ -976,16 +976,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.9897025171624714</v>
+        <v>0.9881769641495042</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9798866615659716</v>
+        <v>0.9883167483262262</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9897025171624714</v>
+        <v>0.9881769641495042</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9847701296895512</v>
+        <v>0.9823006000810917</v>
       </c>
     </row>
     <row r="26">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.9952326468344775</v>
+        <v>0.9956140350877193</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9952553744906822</v>
+        <v>0.9956332717759311</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9952326468344775</v>
+        <v>0.9956140350877193</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9928546657419742</v>
+        <v>0.9934258723732408</v>
       </c>
     </row>
     <row r="27">
@@ -1020,16 +1020,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.990465293668955</v>
+        <v>0.9872234935163997</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9905562042937743</v>
+        <v>0.9873867326343252</v>
       </c>
       <c r="E27" t="n">
-        <v>0.990465293668955</v>
+        <v>0.9872234935163997</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9857207770294218</v>
+        <v>0.9808763124334327</v>
       </c>
     </row>
     <row r="28">
@@ -1042,16 +1042,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.9557589626239512</v>
+        <v>0.9569031273836766</v>
       </c>
       <c r="D28" t="n">
-        <v>0.9480073465504215</v>
+        <v>0.9435498674864152</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9557589626239512</v>
+        <v>0.9569031273836766</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9357494494700589</v>
+        <v>0.9377883522955645</v>
       </c>
     </row>
     <row r="29">
@@ -1064,16 +1064,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.8710907704042715</v>
+        <v>0.8838672768878718</v>
       </c>
       <c r="D29" t="n">
-        <v>0.870557247257468</v>
+        <v>0.8831391013379382</v>
       </c>
       <c r="E29" t="n">
-        <v>0.8710907704042715</v>
+        <v>0.8838672768878718</v>
       </c>
       <c r="F29" t="n">
-        <v>0.864849965500176</v>
+        <v>0.8785273189346098</v>
       </c>
     </row>
     <row r="30">
@@ -1086,16 +1086,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.9464149504195271</v>
+        <v>0.9509916094584286</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9461331094188488</v>
+        <v>0.9496097270464978</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9464149504195271</v>
+        <v>0.9509916094584286</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9367301435516877</v>
+        <v>0.9423296952066764</v>
       </c>
     </row>
     <row r="31">
@@ -1108,16 +1108,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.9315408085430968</v>
+        <v>0.9431731502669718</v>
       </c>
       <c r="D31" t="n">
-        <v>0.9239993681313369</v>
+        <v>0.9376761152443363</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9315408085430968</v>
+        <v>0.9431731502669718</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9219083893364928</v>
+        <v>0.9364232454518965</v>
       </c>
     </row>
     <row r="32">
@@ -1130,16 +1130,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.9912280701754386</v>
+        <v>0.9908466819221968</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9885032654140598</v>
+        <v>0.988001369824934</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9912280701754386</v>
+        <v>0.9908466819221968</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9873869095040725</v>
+        <v>0.9868182720113153</v>
       </c>
     </row>
     <row r="33">
@@ -1152,16 +1152,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.9605263157894737</v>
+        <v>0.9603356216628528</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9586272939750693</v>
+        <v>0.9586697165006033</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9605263157894737</v>
+        <v>0.9603356216628528</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9581335039687298</v>
+        <v>0.957564378312695</v>
       </c>
     </row>
     <row r="34">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.9794050343249427</v>
+        <v>0.9780701754385965</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9798298349920371</v>
+        <v>0.9707901173606633</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9794050343249427</v>
+        <v>0.9780701754385965</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9705435657957914</v>
+        <v>0.9693926683477269</v>
       </c>
     </row>
     <row r="35">
@@ -1196,16 +1196,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.9496567505720824</v>
+        <v>0.948512585812357</v>
       </c>
       <c r="D35" t="n">
-        <v>0.9411202590865966</v>
+        <v>0.9343987420019269</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9496567505720824</v>
+        <v>0.948512585812357</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9267559445026519</v>
+        <v>0.9255903200972527</v>
       </c>
     </row>
     <row r="36">
@@ -1218,16 +1218,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.8775743707093822</v>
+        <v>0.8771929824561403</v>
       </c>
       <c r="D36" t="n">
-        <v>0.8699203147894478</v>
+        <v>0.8700135557593731</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8775743707093822</v>
+        <v>0.8771929824561403</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8666279870380813</v>
+        <v>0.8663009766207301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>